<commit_message>
Function selection of locations
</commit_message>
<xml_diff>
--- a/regression/Plots_PH1_2022-06-10/Regression_parameters.xlsx
+++ b/regression/Plots_PH1_2022-06-10/Regression_parameters.xlsx
@@ -1578,13 +1578,13 @@
         </is>
       </c>
       <c r="AR5" t="n">
-        <v>-4.880510354374826</v>
+        <v>4.059857619533594</v>
       </c>
       <c r="AS5" t="n">
-        <v>12.08767024190333</v>
+        <v>2.861469442540375e-21</v>
       </c>
       <c r="AT5" t="n">
-        <v>1</v>
+        <v>58.90026371088006</v>
       </c>
       <c r="AU5" t="n">
         <v>1</v>
@@ -1616,16 +1616,16 @@
       </c>
       <c r="BE5" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="BH5" t="n">
-        <v>0.886560074781514</v>
+        <v>1.328938288177248</v>
       </c>
     </row>
     <row r="6">
@@ -1753,16 +1753,16 @@
         </is>
       </c>
       <c r="AR6" t="n">
-        <v>92.07995745730085</v>
+        <v>-4.880510354374826</v>
       </c>
       <c r="AS6" t="n">
-        <v>-146.8467431695306</v>
+        <v>12.08767024190333</v>
       </c>
       <c r="AT6" t="n">
-        <v>-97.04584448318346</v>
+        <v>1</v>
       </c>
       <c r="AU6" t="n">
-        <v>164.7737964312615</v>
+        <v>1</v>
       </c>
       <c r="AV6" t="n">
         <v>1</v>
@@ -1791,16 +1791,16 @@
       </c>
       <c r="BE6" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="BF6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="BH6" t="n">
-        <v>0.5046251301584253</v>
+        <v>0.886560074781514</v>
       </c>
     </row>
     <row r="7">
@@ -1928,16 +1928,16 @@
         </is>
       </c>
       <c r="AR7" t="n">
-        <v>0.7338967599833205</v>
+        <v>92.07995745730085</v>
       </c>
       <c r="AS7" t="n">
-        <v>0.1972670261076105</v>
+        <v>-146.8467431695306</v>
       </c>
       <c r="AT7" t="n">
-        <v>3.616928327498513</v>
+        <v>-97.04584448318346</v>
       </c>
       <c r="AU7" t="n">
-        <v>1</v>
+        <v>164.7737964312615</v>
       </c>
       <c r="AV7" t="n">
         <v>1</v>
@@ -1966,16 +1966,16 @@
       </c>
       <c r="BE7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="BF7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="BH7" t="n">
-        <v>0.7902592927374807</v>
+        <v>0.5046251301584253</v>
       </c>
     </row>
     <row r="8">
@@ -2103,22 +2103,22 @@
         </is>
       </c>
       <c r="AR8" t="n">
-        <v>35.75981871605691</v>
+        <v>0.7338967599833205</v>
       </c>
       <c r="AS8" t="n">
-        <v>-52.55576025282894</v>
+        <v>0.1972670261076105</v>
       </c>
       <c r="AT8" t="n">
-        <v>-0.2710479656272216</v>
+        <v>3.616928327498513</v>
       </c>
       <c r="AU8" t="n">
-        <v>1.078950164204641</v>
+        <v>1</v>
       </c>
       <c r="AV8" t="n">
-        <v>-4.749875425753947</v>
+        <v>1</v>
       </c>
       <c r="AW8" t="n">
-        <v>9.866387518845828</v>
+        <v>1</v>
       </c>
       <c r="AX8" t="n">
         <v>1</v>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="BE8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="BF8" t="inlineStr">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="BH8" t="n">
-        <v>0.06273205538254371</v>
+        <v>0.7902592927374807</v>
       </c>
     </row>
     <row r="9">
@@ -2278,22 +2278,22 @@
         </is>
       </c>
       <c r="AR9" t="n">
-        <v>4.4573516854008</v>
+        <v>35.75981871605691</v>
       </c>
       <c r="AS9" t="n">
-        <v>1</v>
+        <v>-52.55576025282894</v>
       </c>
       <c r="AT9" t="n">
-        <v>1</v>
+        <v>-0.2710479656272216</v>
       </c>
       <c r="AU9" t="n">
-        <v>1</v>
+        <v>1.078950164204641</v>
       </c>
       <c r="AV9" t="n">
-        <v>1</v>
+        <v>-4.749875425753947</v>
       </c>
       <c r="AW9" t="n">
-        <v>1</v>
+        <v>9.866387518845828</v>
       </c>
       <c r="AX9" t="n">
         <v>1</v>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="BB9" t="inlineStr">
         <is>
-          <t>tan_phi</t>
+          <t>Dr</t>
         </is>
       </c>
       <c r="BC9" t="inlineStr">
@@ -2316,16 +2316,16 @@
       </c>
       <c r="BE9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="BF9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="BH9" t="n">
-        <v>2.723503620974602</v>
+        <v>0.06273205538254371</v>
       </c>
     </row>
     <row r="10">
@@ -2453,10 +2453,10 @@
         </is>
       </c>
       <c r="AR10" t="n">
-        <v>-90.06936959825512</v>
+        <v>4.4573516854008</v>
       </c>
       <c r="AS10" t="n">
-        <v>166.4826711756099</v>
+        <v>1</v>
       </c>
       <c r="AT10" t="n">
         <v>1</v>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="BE10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="BF10" t="inlineStr">
@@ -2500,7 +2500,7 @@
         </is>
       </c>
       <c r="BH10" t="n">
-        <v>0.2556197613510633</v>
+        <v>2.723503620974602</v>
       </c>
     </row>
     <row r="11">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="AR11" t="n">
-        <v>-4.880510354374826</v>
+        <v>-90.06936959825512</v>
       </c>
       <c r="AS11" t="n">
-        <v>12.08767024190333</v>
+        <v>166.4826711756099</v>
       </c>
       <c r="AT11" t="n">
         <v>1</v>
@@ -2666,16 +2666,16 @@
       </c>
       <c r="BE11" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="BF11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="BH11" t="n">
-        <v>0.886560074781514</v>
+        <v>0.2556197613510633</v>
       </c>
     </row>
     <row r="12">
@@ -2803,16 +2803,16 @@
         </is>
       </c>
       <c r="AR12" t="n">
-        <v>109.3986263993442</v>
+        <v>-0.370730212354445</v>
       </c>
       <c r="AS12" t="n">
-        <v>-190.6770910320547</v>
+        <v>2.703917636572826e-08</v>
       </c>
       <c r="AT12" t="n">
-        <v>-231.3277843654793</v>
+        <v>33.29778267972279</v>
       </c>
       <c r="AU12" t="n">
-        <v>413.4344362464644</v>
+        <v>1</v>
       </c>
       <c r="AV12" t="n">
         <v>1</v>
@@ -2841,16 +2841,16 @@
       </c>
       <c r="BE12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="BF12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="BH12" t="n">
-        <v>0.0814159662904233</v>
+        <v>0.05366138066021946</v>
       </c>
     </row>
     <row r="13">
@@ -2978,13 +2978,13 @@
         </is>
       </c>
       <c r="AR13" t="n">
-        <v>0.7338967599833205</v>
+        <v>-4.880510354374826</v>
       </c>
       <c r="AS13" t="n">
-        <v>0.1972670261076105</v>
+        <v>12.08767024190333</v>
       </c>
       <c r="AT13" t="n">
-        <v>3.616928327498513</v>
+        <v>1</v>
       </c>
       <c r="AU13" t="n">
         <v>1</v>
@@ -3021,11 +3021,11 @@
       </c>
       <c r="BF13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="BH13" t="n">
-        <v>0.7902592927374807</v>
+        <v>0.886560074781514</v>
       </c>
     </row>
     <row r="14">
@@ -3147,6 +3147,61 @@
           <t>B_FC15.1_OCR1_DR69_undrained</t>
         </is>
       </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>Pu</t>
+        </is>
+      </c>
+      <c r="AR14" t="n">
+        <v>109.3986263993442</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>-190.6770910320547</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>-231.3277843654793</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>413.4344362464644</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB14" t="inlineStr">
+        <is>
+          <t>tan_phi</t>
+        </is>
+      </c>
+      <c r="BC14" t="inlineStr">
+        <is>
+          <t>z_L</t>
+        </is>
+      </c>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.0814159662904233</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3266,6 +3321,61 @@
         <is>
           <t>B_FC15.1_OCR1_DR69_undrained</t>
         </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>Pu</t>
+        </is>
+      </c>
+      <c r="AR15" t="n">
+        <v>0.7338967599833205</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0.1972670261076105</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>3.616928327498513</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB15" t="inlineStr">
+        <is>
+          <t>tan_phi</t>
+        </is>
+      </c>
+      <c r="BC15" t="inlineStr">
+        <is>
+          <t>z_L</t>
+        </is>
+      </c>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.7902592927374807</v>
       </c>
     </row>
     <row r="16">

</xml_diff>